<commit_message>
Updated project Feat_ForwardAssignment_Final and fixed sheet logic
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feat Systems\Documents\UiPath\Feat_ForwardAssignment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feat Systems\Documents\UiPath\Feat_ForwardAssignment_Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32744E3-7843-4610-A956-9DFAD8C21DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C784A2E3-4328-4470-AE90-36F7E73C32A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,11 +18,16 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +183,12 @@
   </si>
   <si>
     <t>Workbook3_Path</t>
+  </si>
+  <si>
+    <t>SheetNames</t>
+  </si>
+  <si>
+    <t>AMER HLS,AMER FINS,AMER PORTFOLIO,AMER MEU,AMER COMMERCIAL,AMER PS,APJ,EMEA</t>
   </si>
 </sst>
 </file>
@@ -556,13 +567,13 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -658,7 +669,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1658,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Made changes in config file using assets
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feat Systems\Documents\UiPath\Feat_ForwardAssignment_Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C784A2E3-4328-4470-AE90-36F7E73C32A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1834B7-80F3-48D3-8982-637155DD9D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -189,6 +189,27 @@
   </si>
   <si>
     <t>AMER HLS,AMER FINS,AMER PORTFOLIO,AMER MEU,AMER COMMERCIAL,AMER PS,APJ,EMEA</t>
+  </si>
+  <si>
+    <t>Forward_CompCodeTracker_FilePath</t>
+  </si>
+  <si>
+    <t>CompCodeTracker_FilePath</t>
+  </si>
+  <si>
+    <t>Feat_Forward</t>
+  </si>
+  <si>
+    <t>Forward_COMP Passes Master_FilePath</t>
+  </si>
+  <si>
+    <t>COMP Passes Master_FilePath</t>
+  </si>
+  <si>
+    <t>Forward_FUSIONRegistrationReport_FilePath</t>
+  </si>
+  <si>
+    <t>FUSIONRegistrationReport_FilePath</t>
   </si>
 </sst>
 </file>
@@ -566,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2839,14 +2860,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -2887,9 +2908,39 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3889,5 +3940,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>